<commit_message>
converted all png to bmp
</commit_message>
<xml_diff>
--- a/Resources/map.xlsx
+++ b/Resources/map.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -362,7 +363,7 @@
   <dimension ref="A1:AB60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -464,11 +465,83 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
       <c r="N5" s="1">
         <v>1</v>
       </c>
       <c r="O5" s="1">
         <v>1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0</v>
       </c>
       <c r="AB5" s="1">
         <v>1</v>
@@ -478,6 +551,9 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -490,6 +566,9 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
       <c r="H6" s="1">
         <v>1</v>
       </c>
@@ -505,11 +584,50 @@
       <c r="L6" s="1">
         <v>1</v>
       </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
       <c r="N6" s="1">
         <v>1</v>
       </c>
       <c r="O6" s="1">
         <v>1</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>0</v>
       </c>
       <c r="AB6" s="1">
         <v>1</v>
@@ -519,6 +637,9 @@
       <c r="A7" s="1">
         <v>1</v>
       </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
@@ -531,6 +652,9 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
       <c r="H7" s="1">
         <v>1</v>
       </c>
@@ -546,11 +670,50 @@
       <c r="L7" s="1">
         <v>1</v>
       </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
       <c r="N7" s="1">
         <v>1</v>
       </c>
       <c r="O7" s="1">
         <v>1</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1">
+        <v>1</v>
+      </c>
+      <c r="T7" s="1">
+        <v>1</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0</v>
       </c>
       <c r="AB7" s="1">
         <v>1</v>
@@ -560,6 +723,9 @@
       <c r="A8" s="1">
         <v>1</v>
       </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
@@ -572,6 +738,9 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
       <c r="H8" s="1">
         <v>1</v>
       </c>
@@ -587,11 +756,50 @@
       <c r="L8" s="1">
         <v>1</v>
       </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
       <c r="N8" s="1">
         <v>1</v>
       </c>
       <c r="O8" s="1">
         <v>1</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>1</v>
+      </c>
+      <c r="R8" s="1">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1</v>
+      </c>
+      <c r="T8" s="1">
+        <v>1</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
+        <v>1</v>
+      </c>
+      <c r="X8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0</v>
       </c>
       <c r="AB8" s="1">
         <v>1</v>
@@ -601,6 +809,84 @@
       <c r="A9" s="1">
         <v>1</v>
       </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0</v>
+      </c>
       <c r="AB9" s="1">
         <v>1</v>
       </c>
@@ -609,6 +895,9 @@
       <c r="A10" s="1">
         <v>1</v>
       </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
@@ -621,11 +910,68 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
       <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>1</v>
+      </c>
+      <c r="U10" s="1">
+        <v>1</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0</v>
+      </c>
+      <c r="W10" s="1">
+        <v>1</v>
+      </c>
+      <c r="X10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0</v>
       </c>
       <c r="AB10" s="1">
         <v>1</v>
@@ -635,6 +981,9 @@
       <c r="A11" s="1">
         <v>1</v>
       </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
@@ -647,11 +996,68 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
       <c r="H11" s="1">
         <v>1</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>1</v>
+      </c>
+      <c r="R11" s="1">
+        <v>1</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1">
+        <v>1</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0</v>
+      </c>
+      <c r="W11" s="1">
+        <v>1</v>
+      </c>
+      <c r="X11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0</v>
       </c>
       <c r="AB11" s="1">
         <v>1</v>
@@ -661,11 +1067,83 @@
       <c r="A12" s="1">
         <v>1</v>
       </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
       <c r="H12" s="1">
         <v>1</v>
       </c>
       <c r="I12" s="1">
         <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
+        <v>1</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1">
+        <v>1</v>
+      </c>
+      <c r="U12" s="1">
+        <v>1</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>0</v>
       </c>
       <c r="AB12" s="1">
         <v>1</v>
@@ -690,6 +1168,9 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
       <c r="H13" s="1">
         <v>1</v>
       </c>
@@ -704,6 +1185,36 @@
       </c>
       <c r="L13" s="1">
         <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1">
+        <v>1</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1">
+        <v>1</v>
+      </c>
+      <c r="T13" s="1">
+        <v>1</v>
+      </c>
+      <c r="U13" s="1">
+        <v>1</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0</v>
       </c>
       <c r="W13" s="1">
         <v>1</v>
@@ -743,6 +1254,9 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
       <c r="H14" s="1">
         <v>1</v>
       </c>
@@ -757,6 +1271,36 @@
       </c>
       <c r="L14" s="1">
         <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1">
+        <v>1</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>1</v>
+      </c>
+      <c r="R14" s="1">
+        <v>1</v>
+      </c>
+      <c r="S14" s="1">
+        <v>1</v>
+      </c>
+      <c r="T14" s="1">
+        <v>1</v>
+      </c>
+      <c r="U14" s="1">
+        <v>1</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0</v>
       </c>
       <c r="W14" s="1">
         <v>1</v>
@@ -796,11 +1340,53 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
       <c r="H15" s="1">
         <v>1</v>
       </c>
       <c r="I15" s="1">
         <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1">
+        <v>1</v>
+      </c>
+      <c r="U15" s="1">
+        <v>1</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0</v>
       </c>
       <c r="W15" s="1">
         <v>1</v>
@@ -840,11 +1426,17 @@
       <c r="F16" s="1">
         <v>1</v>
       </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
       <c r="H16" s="1">
         <v>1</v>
       </c>
       <c r="I16" s="1">
         <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
       </c>
       <c r="N16" s="1">
         <v>3</v>
@@ -852,6 +1444,15 @@
       <c r="O16" s="1">
         <v>3</v>
       </c>
+      <c r="T16" s="1">
+        <v>1</v>
+      </c>
+      <c r="U16" s="1">
+        <v>1</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0</v>
+      </c>
       <c r="W16" s="1">
         <v>1</v>
       </c>
@@ -890,11 +1491,26 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
       <c r="H17" s="1">
         <v>1</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1">
+        <v>1</v>
+      </c>
+      <c r="U17" s="1">
+        <v>1</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0</v>
       </c>
       <c r="W17" s="1">
         <v>1</v>
@@ -919,6 +1535,51 @@
       <c r="A18" s="1">
         <v>2</v>
       </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="V18" s="1">
+        <v>0</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0</v>
+      </c>
+      <c r="X18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>0</v>
+      </c>
       <c r="AB18" s="1">
         <v>2</v>
       </c>
@@ -942,6 +1603,12 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="V19" s="1">
+        <v>0</v>
+      </c>
       <c r="W19" s="1">
         <v>1</v>
       </c>
@@ -980,6 +1647,12 @@
       <c r="F20" s="1">
         <v>1</v>
       </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0</v>
+      </c>
       <c r="W20" s="1">
         <v>1</v>
       </c>
@@ -1018,6 +1691,12 @@
       <c r="F21" s="1">
         <v>1</v>
       </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0</v>
+      </c>
       <c r="W21" s="1">
         <v>1</v>
       </c>
@@ -1056,6 +1735,36 @@
       <c r="F22" s="1">
         <v>1</v>
       </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1">
+        <v>1</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1">
+        <v>1</v>
+      </c>
+      <c r="V22" s="1">
+        <v>0</v>
+      </c>
       <c r="W22" s="1">
         <v>1</v>
       </c>
@@ -1094,6 +1803,36 @@
       <c r="F23" s="1">
         <v>1</v>
       </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1">
+        <v>1</v>
+      </c>
+      <c r="P23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1">
+        <v>1</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0</v>
+      </c>
       <c r="W23" s="1">
         <v>1</v>
       </c>
@@ -1117,6 +1856,39 @@
       <c r="A24" s="1">
         <v>1</v>
       </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1">
+        <v>1</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="V24" s="1">
+        <v>0</v>
+      </c>
       <c r="AB24" s="1">
         <v>1</v>
       </c>
@@ -1137,6 +1909,9 @@
       <c r="F25" s="1">
         <v>1</v>
       </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
       <c r="H25" s="1">
         <v>1</v>
       </c>
@@ -1151,6 +1926,36 @@
       </c>
       <c r="L25" s="1">
         <v>1</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1">
+        <v>1</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1">
+        <v>1</v>
+      </c>
+      <c r="S25" s="1">
+        <v>1</v>
+      </c>
+      <c r="T25" s="1">
+        <v>1</v>
+      </c>
+      <c r="U25" s="1">
+        <v>1</v>
+      </c>
+      <c r="V25" s="1">
+        <v>0</v>
       </c>
       <c r="AB25" s="1">
         <v>1</v>
@@ -1172,6 +1977,9 @@
       <c r="F26" s="1">
         <v>1</v>
       </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
       <c r="H26" s="1">
         <v>1</v>
       </c>
@@ -1186,6 +1994,36 @@
       </c>
       <c r="L26" s="1">
         <v>1</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1">
+        <v>1</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1">
+        <v>1</v>
+      </c>
+      <c r="S26" s="1">
+        <v>1</v>
+      </c>
+      <c r="T26" s="1">
+        <v>1</v>
+      </c>
+      <c r="U26" s="1">
+        <v>1</v>
+      </c>
+      <c r="V26" s="1">
+        <v>0</v>
       </c>
       <c r="AB26" s="1">
         <v>1</v>
@@ -1201,6 +2039,54 @@
       <c r="F27" s="1">
         <v>1</v>
       </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0</v>
+      </c>
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>0</v>
+      </c>
+      <c r="R27" s="1">
+        <v>0</v>
+      </c>
+      <c r="S27" s="1">
+        <v>0</v>
+      </c>
+      <c r="T27" s="1">
+        <v>0</v>
+      </c>
+      <c r="U27" s="1">
+        <v>0</v>
+      </c>
+      <c r="V27" s="1">
+        <v>0</v>
+      </c>
       <c r="AB27" s="1">
         <v>1</v>
       </c>
@@ -1221,6 +2107,9 @@
       <c r="F28" s="1">
         <v>1</v>
       </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
       <c r="H28" s="1">
         <v>1</v>
       </c>
@@ -1253,6 +2142,9 @@
       <c r="F29" s="1">
         <v>1</v>
       </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
       <c r="H29" s="1">
         <v>1</v>
       </c>
@@ -1273,6 +2165,9 @@
       <c r="A30" s="1">
         <v>1</v>
       </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
       <c r="H30" s="1">
         <v>1</v>
       </c>
@@ -1315,6 +2210,9 @@
         <v>1</v>
       </c>
       <c r="L31" s="1">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1">
         <v>1</v>
       </c>
       <c r="AB31" s="1">
@@ -1485,4 +2383,1131 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <picture r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB58"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="54" width="2.21875" style="1" customWidth="1"/>
+    <col min="55" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1">
+        <v>1</v>
+      </c>
+      <c r="S1" s="1">
+        <v>1</v>
+      </c>
+      <c r="T1" s="1">
+        <v>1</v>
+      </c>
+      <c r="U1" s="1">
+        <v>1</v>
+      </c>
+      <c r="V1" s="1">
+        <v>1</v>
+      </c>
+      <c r="W1" s="1">
+        <v>1</v>
+      </c>
+      <c r="X1" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="W10" s="1">
+        <v>1</v>
+      </c>
+      <c r="X10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="W11" s="1">
+        <v>1</v>
+      </c>
+      <c r="X11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="W12" s="1">
+        <v>1</v>
+      </c>
+      <c r="X12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>3</v>
+      </c>
+      <c r="O13" s="1">
+        <v>3</v>
+      </c>
+      <c r="W13" s="1">
+        <v>1</v>
+      </c>
+      <c r="X13" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="W14" s="1">
+        <v>1</v>
+      </c>
+      <c r="X14" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="W16" s="1">
+        <v>1</v>
+      </c>
+      <c r="X16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="W17" s="1">
+        <v>1</v>
+      </c>
+      <c r="X17" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="W18" s="1">
+        <v>1</v>
+      </c>
+      <c r="X18" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="W19" s="1">
+        <v>1</v>
+      </c>
+      <c r="X19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="W20" s="1">
+        <v>1</v>
+      </c>
+      <c r="X20" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="1">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1">
+        <v>1</v>
+      </c>
+      <c r="P31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1">
+        <v>1</v>
+      </c>
+      <c r="S31" s="1">
+        <v>1</v>
+      </c>
+      <c r="T31" s="1">
+        <v>1</v>
+      </c>
+      <c r="U31" s="1">
+        <v>1</v>
+      </c>
+      <c r="V31" s="1">
+        <v>1</v>
+      </c>
+      <c r="W31" s="1">
+        <v>1</v>
+      </c>
+      <c r="X31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="15.6" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working on collision detect
</commit_message>
<xml_diff>
--- a/Resources/map.xlsx
+++ b/Resources/map.xlsx
@@ -363,7 +363,7 @@
   <dimension ref="A1:AB60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1438,12 +1438,33 @@
       <c r="J16" s="1">
         <v>0</v>
       </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
       <c r="N16" s="1">
         <v>3</v>
       </c>
       <c r="O16" s="1">
         <v>3</v>
       </c>
+      <c r="P16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+      <c r="R16" s="1">
+        <v>1</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
       <c r="T16" s="1">
         <v>1</v>
       </c>
@@ -1501,6 +1522,33 @@
         <v>1</v>
       </c>
       <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1">
+        <v>1</v>
+      </c>
+      <c r="S17" s="1">
         <v>0</v>
       </c>
       <c r="T17" s="1">
@@ -1536,19 +1584,19 @@
         <v>2</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
@@ -1562,23 +1610,56 @@
       <c r="J18" s="1">
         <v>0</v>
       </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1">
+        <v>1</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0</v>
+      </c>
+      <c r="U18" s="1">
+        <v>0</v>
+      </c>
       <c r="V18" s="1">
         <v>0</v>
       </c>
       <c r="W18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB18" s="1">
         <v>2</v>
@@ -1606,6 +1687,48 @@
       <c r="G19" s="1">
         <v>0</v>
       </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1">
+        <v>1</v>
+      </c>
+      <c r="S19" s="1">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1">
+        <v>1</v>
+      </c>
+      <c r="U19" s="1">
+        <v>1</v>
+      </c>
       <c r="V19" s="1">
         <v>0</v>
       </c>
@@ -1650,6 +1773,48 @@
       <c r="G20" s="1">
         <v>0</v>
       </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1">
+        <v>1</v>
+      </c>
+      <c r="P20" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>1</v>
+      </c>
+      <c r="R20" s="1">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1">
+        <v>1</v>
+      </c>
+      <c r="U20" s="1">
+        <v>1</v>
+      </c>
       <c r="V20" s="1">
         <v>0</v>
       </c>
@@ -1694,6 +1859,48 @@
       <c r="G21" s="1">
         <v>0</v>
       </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+      <c r="T21" s="1">
+        <v>1</v>
+      </c>
+      <c r="U21" s="1">
+        <v>1</v>
+      </c>
       <c r="V21" s="1">
         <v>0</v>
       </c>
@@ -1738,6 +1945,15 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
       <c r="K22" s="1">
         <v>1</v>
       </c>
@@ -1760,6 +1976,15 @@
         <v>1</v>
       </c>
       <c r="R22" s="1">
+        <v>1</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1">
+        <v>1</v>
+      </c>
+      <c r="U22" s="1">
         <v>1</v>
       </c>
       <c r="V22" s="1">
@@ -1806,6 +2031,15 @@
       <c r="G23" s="1">
         <v>0</v>
       </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
       <c r="K23" s="1">
         <v>1</v>
       </c>
@@ -1828,6 +2062,15 @@
         <v>1</v>
       </c>
       <c r="R23" s="1">
+        <v>1</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1">
+        <v>1</v>
+      </c>
+      <c r="U23" s="1">
         <v>1</v>
       </c>
       <c r="V23" s="1">
@@ -1856,6 +2099,21 @@
       <c r="A24" s="1">
         <v>1</v>
       </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
       <c r="G24" s="1">
         <v>0</v>
       </c>
@@ -1886,7 +2144,37 @@
       <c r="P24" s="1">
         <v>0</v>
       </c>
+      <c r="Q24" s="1">
+        <v>0</v>
+      </c>
+      <c r="R24" s="1">
+        <v>0</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24" s="1">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1">
+        <v>0</v>
+      </c>
       <c r="V24" s="1">
+        <v>0</v>
+      </c>
+      <c r="W24" s="1">
+        <v>0</v>
+      </c>
+      <c r="X24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="1">
         <v>0</v>
       </c>
       <c r="AB24" s="1">
@@ -1897,6 +2185,9 @@
       <c r="A25" s="1">
         <v>1</v>
       </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
@@ -1955,6 +2246,21 @@
         <v>1</v>
       </c>
       <c r="V25" s="1">
+        <v>0</v>
+      </c>
+      <c r="W25" s="1">
+        <v>1</v>
+      </c>
+      <c r="X25" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="1">
         <v>0</v>
       </c>
       <c r="AB25" s="1">
@@ -1965,6 +2271,9 @@
       <c r="A26" s="1">
         <v>1</v>
       </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
@@ -2023,6 +2332,21 @@
         <v>1</v>
       </c>
       <c r="V26" s="1">
+        <v>0</v>
+      </c>
+      <c r="W26" s="1">
+        <v>1</v>
+      </c>
+      <c r="X26" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="1">
         <v>0</v>
       </c>
       <c r="AB26" s="1">
@@ -2033,6 +2357,15 @@
       <c r="A27" s="1">
         <v>1</v>
       </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
@@ -2085,6 +2418,21 @@
         <v>0</v>
       </c>
       <c r="V27" s="1">
+        <v>0</v>
+      </c>
+      <c r="W27" s="1">
+        <v>1</v>
+      </c>
+      <c r="X27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1">
         <v>0</v>
       </c>
       <c r="AB27" s="1">
@@ -2101,6 +2449,9 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
       <c r="E28" s="1">
         <v>1</v>
       </c>
@@ -2115,6 +2466,54 @@
       </c>
       <c r="I28" s="1">
         <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1">
+        <v>1</v>
+      </c>
+      <c r="N28" s="1">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1">
+        <v>1</v>
+      </c>
+      <c r="P28" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>1</v>
+      </c>
+      <c r="R28" s="1">
+        <v>1</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1">
+        <v>1</v>
+      </c>
+      <c r="U28" s="1">
+        <v>1</v>
+      </c>
+      <c r="V28" s="1">
+        <v>0</v>
+      </c>
+      <c r="W28" s="1">
+        <v>1</v>
+      </c>
+      <c r="X28" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>0</v>
       </c>
       <c r="Z28" s="1">
         <v>1</v>
@@ -2136,6 +2535,9 @@
       <c r="C29" s="1">
         <v>1</v>
       </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
       <c r="E29" s="1">
         <v>1</v>
       </c>
@@ -2150,6 +2552,54 @@
       </c>
       <c r="I29" s="1">
         <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1</v>
+      </c>
+      <c r="M29" s="1">
+        <v>1</v>
+      </c>
+      <c r="N29" s="1">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1">
+        <v>1</v>
+      </c>
+      <c r="P29" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>1</v>
+      </c>
+      <c r="R29" s="1">
+        <v>1</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1">
+        <v>1</v>
+      </c>
+      <c r="U29" s="1">
+        <v>1</v>
+      </c>
+      <c r="V29" s="1">
+        <v>0</v>
+      </c>
+      <c r="W29" s="1">
+        <v>1</v>
+      </c>
+      <c r="X29" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>0</v>
       </c>
       <c r="Z29" s="1">
         <v>1</v>
@@ -2165,6 +2615,21 @@
       <c r="A30" s="1">
         <v>1</v>
       </c>
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
       <c r="G30" s="1">
         <v>0</v>
       </c>
@@ -2173,6 +2638,60 @@
       </c>
       <c r="I30" s="1">
         <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1">
+        <v>1</v>
+      </c>
+      <c r="P30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0</v>
+      </c>
+      <c r="R30" s="1">
+        <v>0</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0</v>
+      </c>
+      <c r="T30" s="1">
+        <v>1</v>
+      </c>
+      <c r="U30" s="1">
+        <v>1</v>
+      </c>
+      <c r="V30" s="1">
+        <v>0</v>
+      </c>
+      <c r="W30" s="1">
+        <v>0</v>
+      </c>
+      <c r="X30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>0</v>
       </c>
       <c r="AB30" s="1">
         <v>1</v>
@@ -2182,6 +2701,9 @@
       <c r="A31" s="1">
         <v>1</v>
       </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
@@ -2212,8 +2734,50 @@
       <c r="L31" s="1">
         <v>1</v>
       </c>
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1">
+        <v>1</v>
+      </c>
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
       <c r="R31" s="1">
         <v>1</v>
+      </c>
+      <c r="S31" s="1">
+        <v>1</v>
+      </c>
+      <c r="T31" s="1">
+        <v>1</v>
+      </c>
+      <c r="U31" s="1">
+        <v>1</v>
+      </c>
+      <c r="V31" s="1">
+        <v>1</v>
+      </c>
+      <c r="W31" s="1">
+        <v>1</v>
+      </c>
+      <c r="X31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>0</v>
       </c>
       <c r="AB31" s="1">
         <v>1</v>
@@ -2223,6 +2787,9 @@
       <c r="A32" s="1">
         <v>1</v>
       </c>
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
@@ -2252,6 +2819,51 @@
       </c>
       <c r="L32" s="1">
         <v>1</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1">
+        <v>1</v>
+      </c>
+      <c r="O32" s="1">
+        <v>1</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>1</v>
+      </c>
+      <c r="R32" s="1">
+        <v>1</v>
+      </c>
+      <c r="S32" s="1">
+        <v>1</v>
+      </c>
+      <c r="T32" s="1">
+        <v>1</v>
+      </c>
+      <c r="U32" s="1">
+        <v>1</v>
+      </c>
+      <c r="V32" s="1">
+        <v>1</v>
+      </c>
+      <c r="W32" s="1">
+        <v>1</v>
+      </c>
+      <c r="X32" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>0</v>
       </c>
       <c r="AB32" s="1">
         <v>1</v>
@@ -2260,6 +2872,84 @@
     <row r="33" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>1</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0</v>
+      </c>
+      <c r="R33" s="1">
+        <v>0</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1">
+        <v>0</v>
+      </c>
+      <c r="U33" s="1">
+        <v>0</v>
+      </c>
+      <c r="V33" s="1">
+        <v>0</v>
+      </c>
+      <c r="W33" s="1">
+        <v>0</v>
+      </c>
+      <c r="X33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>0</v>
       </c>
       <c r="AB33" s="1">
         <v>1</v>
@@ -2387,13 +3077,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB58"/>
+  <dimension ref="A1:AB57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="54" width="2.21875" style="1" customWidth="1"/>
     <col min="55" max="16384" width="8.88671875" style="1"/>
@@ -3504,7 +4194,6 @@
     <row r="55" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="56" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="57" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on points showing and eaten
暫時能動, 但要再修改overlap判定方式
</commit_message>
<xml_diff>
--- a/Resources/map.xlsx
+++ b/Resources/map.xlsx
@@ -26,7 +26,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -46,6 +46,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="136"/>
@@ -73,11 +81,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -363,7 +374,7 @@
   <dimension ref="A1:AB60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO22" sqref="AO21:AO22"/>
+      <selection activeCell="N27" sqref="N27:O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1426,46 +1437,46 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
-        <v>1</v>
-      </c>
-      <c r="K13" s="1">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1">
-        <v>1</v>
-      </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
-        <v>1</v>
-      </c>
-      <c r="O13" s="1">
-        <v>1</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>1</v>
-      </c>
-      <c r="R13" s="1">
-        <v>1</v>
-      </c>
-      <c r="S13" s="1">
-        <v>1</v>
-      </c>
-      <c r="T13" s="1">
-        <v>1</v>
-      </c>
-      <c r="U13" s="1">
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2">
+        <v>1</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2">
+        <v>1</v>
+      </c>
+      <c r="S13" s="2">
+        <v>1</v>
+      </c>
+      <c r="T13" s="2">
+        <v>1</v>
+      </c>
+      <c r="U13" s="2">
         <v>1</v>
       </c>
       <c r="V13" s="1">
@@ -1512,46 +1523,46 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1">
-        <v>1</v>
-      </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>1</v>
-      </c>
-      <c r="O14" s="1">
-        <v>1</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>1</v>
-      </c>
-      <c r="R14" s="1">
-        <v>1</v>
-      </c>
-      <c r="S14" s="1">
-        <v>1</v>
-      </c>
-      <c r="T14" s="1">
-        <v>1</v>
-      </c>
-      <c r="U14" s="1">
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1</v>
+      </c>
+      <c r="S14" s="2">
+        <v>1</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1</v>
+      </c>
+      <c r="U14" s="2">
         <v>1</v>
       </c>
       <c r="V14" s="1">
@@ -1598,46 +1609,46 @@
       <c r="G15" s="1">
         <v>0</v>
       </c>
-      <c r="H15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1">
-        <v>1</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>0</v>
-      </c>
-      <c r="R15" s="1">
-        <v>0</v>
-      </c>
-      <c r="S15" s="1">
-        <v>0</v>
-      </c>
-      <c r="T15" s="1">
-        <v>1</v>
-      </c>
-      <c r="U15" s="1">
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>1</v>
+      </c>
+      <c r="U15" s="2">
         <v>1</v>
       </c>
       <c r="V15" s="1">
@@ -1684,46 +1695,46 @@
       <c r="G16" s="1">
         <v>0</v>
       </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>1</v>
-      </c>
-      <c r="L16" s="1">
-        <v>1</v>
-      </c>
-      <c r="M16" s="1">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1">
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2">
         <v>3</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="2">
         <v>3</v>
       </c>
-      <c r="P16" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>1</v>
-      </c>
-      <c r="R16" s="1">
-        <v>1</v>
-      </c>
-      <c r="S16" s="1">
-        <v>0</v>
-      </c>
-      <c r="T16" s="1">
-        <v>1</v>
-      </c>
-      <c r="U16" s="1">
+      <c r="P16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2">
+        <v>1</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2">
+        <v>1</v>
+      </c>
+      <c r="U16" s="2">
         <v>1</v>
       </c>
       <c r="V16" s="1">
@@ -1770,46 +1781,46 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
-        <v>1</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
         <v>4</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="2">
         <v>4</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N17" s="2">
         <v>4</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17" s="2">
         <v>4</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P17" s="2">
         <v>4</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="Q17" s="2">
         <v>4</v>
       </c>
-      <c r="R17" s="1">
-        <v>1</v>
-      </c>
-      <c r="S17" s="1">
-        <v>0</v>
-      </c>
-      <c r="T17" s="1">
-        <v>1</v>
-      </c>
-      <c r="U17" s="1">
+      <c r="R17" s="2">
+        <v>1</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2">
+        <v>1</v>
+      </c>
+      <c r="U17" s="2">
         <v>1</v>
       </c>
       <c r="V17" s="1">
@@ -1856,46 +1867,46 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
-      <c r="L18" s="1">
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
         <v>4</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18" s="2">
         <v>4</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N18" s="2">
         <v>4</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O18" s="2">
         <v>4</v>
       </c>
-      <c r="P18" s="1">
+      <c r="P18" s="2">
         <v>4</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="Q18" s="2">
         <v>4</v>
       </c>
-      <c r="R18" s="1">
-        <v>1</v>
-      </c>
-      <c r="S18" s="1">
-        <v>0</v>
-      </c>
-      <c r="T18" s="1">
-        <v>0</v>
-      </c>
-      <c r="U18" s="1">
+      <c r="R18" s="2">
+        <v>1</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2">
+        <v>0</v>
+      </c>
+      <c r="U18" s="2">
         <v>0</v>
       </c>
       <c r="V18" s="1">
@@ -1942,46 +1953,46 @@
       <c r="G19" s="1">
         <v>0</v>
       </c>
-      <c r="H19" s="1">
-        <v>1</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1">
-        <v>0</v>
-      </c>
-      <c r="K19" s="1">
-        <v>1</v>
-      </c>
-      <c r="L19" s="1">
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
         <v>4</v>
       </c>
-      <c r="M19" s="1">
+      <c r="M19" s="2">
         <v>4</v>
       </c>
-      <c r="N19" s="1">
+      <c r="N19" s="2">
         <v>4</v>
       </c>
-      <c r="O19" s="1">
+      <c r="O19" s="2">
         <v>4</v>
       </c>
-      <c r="P19" s="1">
+      <c r="P19" s="2">
         <v>4</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="Q19" s="2">
         <v>4</v>
       </c>
-      <c r="R19" s="1">
-        <v>1</v>
-      </c>
-      <c r="S19" s="1">
-        <v>0</v>
-      </c>
-      <c r="T19" s="1">
-        <v>1</v>
-      </c>
-      <c r="U19" s="1">
+      <c r="R19" s="2">
+        <v>1</v>
+      </c>
+      <c r="S19" s="2">
+        <v>0</v>
+      </c>
+      <c r="T19" s="2">
+        <v>1</v>
+      </c>
+      <c r="U19" s="2">
         <v>1</v>
       </c>
       <c r="V19" s="1">
@@ -2028,46 +2039,46 @@
       <c r="G20" s="1">
         <v>0</v>
       </c>
-      <c r="H20" s="1">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1">
-        <v>1</v>
-      </c>
-      <c r="J20" s="1">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1">
-        <v>1</v>
-      </c>
-      <c r="L20" s="1">
-        <v>1</v>
-      </c>
-      <c r="M20" s="1">
-        <v>1</v>
-      </c>
-      <c r="N20" s="1">
-        <v>1</v>
-      </c>
-      <c r="O20" s="1">
-        <v>1</v>
-      </c>
-      <c r="P20" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>1</v>
-      </c>
-      <c r="R20" s="1">
-        <v>1</v>
-      </c>
-      <c r="S20" s="1">
-        <v>0</v>
-      </c>
-      <c r="T20" s="1">
-        <v>1</v>
-      </c>
-      <c r="U20" s="1">
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1</v>
+      </c>
+      <c r="P20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>1</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
+      <c r="S20" s="2">
+        <v>0</v>
+      </c>
+      <c r="T20" s="2">
+        <v>1</v>
+      </c>
+      <c r="U20" s="2">
         <v>1</v>
       </c>
       <c r="V20" s="1">
@@ -2114,46 +2125,46 @@
       <c r="G21" s="1">
         <v>0</v>
       </c>
-      <c r="H21" s="1">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1">
-        <v>1</v>
-      </c>
-      <c r="J21" s="1">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1">
-        <v>0</v>
-      </c>
-      <c r="L21" s="1">
-        <v>0</v>
-      </c>
-      <c r="M21" s="1">
-        <v>0</v>
-      </c>
-      <c r="N21" s="1">
-        <v>0</v>
-      </c>
-      <c r="O21" s="1">
-        <v>0</v>
-      </c>
-      <c r="P21" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>0</v>
-      </c>
-      <c r="R21" s="1">
-        <v>0</v>
-      </c>
-      <c r="S21" s="1">
-        <v>0</v>
-      </c>
-      <c r="T21" s="1">
-        <v>1</v>
-      </c>
-      <c r="U21" s="1">
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>0</v>
+      </c>
+      <c r="R21" s="2">
+        <v>0</v>
+      </c>
+      <c r="S21" s="2">
+        <v>0</v>
+      </c>
+      <c r="T21" s="2">
+        <v>1</v>
+      </c>
+      <c r="U21" s="2">
         <v>1</v>
       </c>
       <c r="V21" s="1">
@@ -2200,46 +2211,46 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1</v>
-      </c>
-      <c r="J22" s="1">
-        <v>0</v>
-      </c>
-      <c r="K22" s="1">
-        <v>1</v>
-      </c>
-      <c r="L22" s="1">
-        <v>1</v>
-      </c>
-      <c r="M22" s="1">
-        <v>1</v>
-      </c>
-      <c r="N22" s="1">
-        <v>1</v>
-      </c>
-      <c r="O22" s="1">
-        <v>1</v>
-      </c>
-      <c r="P22" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>1</v>
-      </c>
-      <c r="R22" s="1">
-        <v>1</v>
-      </c>
-      <c r="S22" s="1">
-        <v>0</v>
-      </c>
-      <c r="T22" s="1">
-        <v>1</v>
-      </c>
-      <c r="U22" s="1">
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2">
+        <v>1</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1</v>
+      </c>
+      <c r="O22" s="2">
+        <v>1</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1</v>
+      </c>
+      <c r="R22" s="2">
+        <v>1</v>
+      </c>
+      <c r="S22" s="2">
+        <v>0</v>
+      </c>
+      <c r="T22" s="2">
+        <v>1</v>
+      </c>
+      <c r="U22" s="2">
         <v>1</v>
       </c>
       <c r="V22" s="1">
@@ -2286,46 +2297,46 @@
       <c r="G23" s="1">
         <v>0</v>
       </c>
-      <c r="H23" s="1">
-        <v>1</v>
-      </c>
-      <c r="I23" s="1">
-        <v>1</v>
-      </c>
-      <c r="J23" s="1">
-        <v>0</v>
-      </c>
-      <c r="K23" s="1">
-        <v>1</v>
-      </c>
-      <c r="L23" s="1">
-        <v>1</v>
-      </c>
-      <c r="M23" s="1">
-        <v>1</v>
-      </c>
-      <c r="N23" s="1">
-        <v>1</v>
-      </c>
-      <c r="O23" s="1">
-        <v>1</v>
-      </c>
-      <c r="P23" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>1</v>
-      </c>
-      <c r="R23" s="1">
-        <v>1</v>
-      </c>
-      <c r="S23" s="1">
-        <v>0</v>
-      </c>
-      <c r="T23" s="1">
-        <v>1</v>
-      </c>
-      <c r="U23" s="1">
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0</v>
+      </c>
+      <c r="T23" s="2">
+        <v>1</v>
+      </c>
+      <c r="U23" s="2">
         <v>1</v>
       </c>
       <c r="V23" s="1">

</xml_diff>